<commit_message>
ajout de la fonction de gestion des équipements
</commit_message>
<xml_diff>
--- a/AutosurveillanceTemplates/PREL.xlsx
+++ b/AutosurveillanceTemplates/PREL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndhuy\AppData\Roaming\Microsoft\AddIns\AutosurveillanceTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11D7B24-D8C6-40E5-84E4-CA8257A9203F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD577D6-CB37-46F6-BD97-37452DD3D395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="3135" windowWidth="29040" windowHeight="15720" tabRatio="777" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1526" uniqueCount="402">
   <si>
     <t>REX des controleurs</t>
   </si>
@@ -2996,9 +2996,6 @@
   </si>
   <si>
     <t>Analyses rendues sous agrément du ministère de l'environnement</t>
-  </si>
-  <si>
-    <t>Code SANDRE :</t>
   </si>
   <si>
     <t xml:space="preserve">Etablissement Concentration
@@ -9362,6 +9359,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="66" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -9683,10 +9684,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -17745,7 +17742,7 @@
         <v>251</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>252</v>
@@ -17831,7 +17828,7 @@
         <v>157</v>
       </c>
       <c r="C4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>255</v>
@@ -17851,11 +17848,11 @@
       <c r="I4" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="O4" s="923" t="str">
+      <c r="O4" s="924" t="str">
         <f ca="1">IF(COUNTIF(R3:AC4,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R3:AC4,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R3:AC4,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R3:AC4,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P4" s="925"/>
+      <c r="P4" s="926"/>
       <c r="Q4" s="20" t="s">
         <v>33</v>
       </c>
@@ -17916,7 +17913,7 @@
         <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>134</v>
@@ -17949,7 +17946,7 @@
         <v>159</v>
       </c>
       <c r="C6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D6" s="114" t="s">
         <v>125</v>
@@ -18037,11 +18034,11 @@
       <c r="I7" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="O7" s="923" t="str">
+      <c r="O7" s="924" t="str">
         <f ca="1">IF(COUNTIF(R6:AC7,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R6:AC7,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R6:AC7,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R6:AC7,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P7" s="924"/>
+      <c r="P7" s="925"/>
       <c r="Q7" s="19" t="s">
         <v>33</v>
       </c>
@@ -18195,11 +18192,11 @@
       <c r="I10" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="O10" s="923" t="str">
+      <c r="O10" s="924" t="str">
         <f ca="1">IF(COUNTIF(R9:AC10,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R9:AC10,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R9:AC10,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R9:AC10,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P10" s="924"/>
+      <c r="P10" s="925"/>
       <c r="Q10" s="19" t="s">
         <v>33</v>
       </c>
@@ -18343,11 +18340,11 @@
       <c r="I13" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="O13" s="923" t="str">
+      <c r="O13" s="924" t="str">
         <f ca="1">IF(COUNTIF(R12:AC13,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R12:AC13,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R12:AC13,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R12:AC13,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P13" s="924"/>
+      <c r="P13" s="925"/>
       <c r="Q13" s="19" t="s">
         <v>33</v>
       </c>
@@ -18488,11 +18485,11 @@
       <c r="I16" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="O16" s="923" t="str">
+      <c r="O16" s="924" t="str">
         <f ca="1">IF(COUNTIF(R15:AC16,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R15:AC16,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R15:AC16,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R15:AC16,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P16" s="924"/>
+      <c r="P16" s="925"/>
       <c r="Q16" s="19" t="s">
         <v>33</v>
       </c>
@@ -18627,11 +18624,11 @@
       <c r="I19" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="O19" s="923" t="str">
+      <c r="O19" s="924" t="str">
         <f ca="1">IF(COUNTIF(R18:AC19,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R18:AC19,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R18:AC19,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R18:AC19,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P19" s="924"/>
+      <c r="P19" s="925"/>
       <c r="Q19" s="19" t="s">
         <v>33</v>
       </c>
@@ -18796,11 +18793,11 @@
         <v>281</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="O22" s="923" t="str">
+      <c r="O22" s="924" t="str">
         <f ca="1">IF(COUNTIF(R21:AC22,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R21:AC22,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R21:AC22,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R21:AC22,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P22" s="924"/>
+      <c r="P22" s="925"/>
       <c r="Q22" s="19" t="s">
         <v>33</v>
       </c>
@@ -18957,11 +18954,11 @@
       <c r="D25" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="O25" s="923" t="str">
+      <c r="O25" s="924" t="str">
         <f ca="1">IF(COUNTIF(R24:AC25,"Non validé par absence d'équipement")&gt;0,"Non validé",IF(COUNTIF(R24:AC25,"Non validé")&gt;0,"Non validé",IF(COUNTIF(R24:AC25,"Validé avec réserve")&gt;0,"Validé avec réserve",IF(COUNTIF(R24:AC25,"Validé")&gt;0,"Validé",""))))</f>
         <v/>
       </c>
-      <c r="P25" s="924"/>
+      <c r="P25" s="925"/>
       <c r="Q25" s="19" t="s">
         <v>33</v>
       </c>
@@ -19131,11 +19128,11 @@
       <c r="N28" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O28" s="923" t="str">
+      <c r="O28" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD27:AD28),0),"")</f>
         <v/>
       </c>
-      <c r="P28" s="924"/>
+      <c r="P28" s="925"/>
       <c r="Q28" s="108" t="s">
         <v>33</v>
       </c>
@@ -19197,11 +19194,11 @@
       <c r="N29" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O29" s="921" t="str">
+      <c r="O29" s="922" t="str">
         <f ca="1">IF(O28="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD27,AD28,AD29),0),TRUNC(AVERAGE(AD27,AD28,AD29),0)))</f>
         <v/>
       </c>
-      <c r="P29" s="926"/>
+      <c r="P29" s="927"/>
       <c r="Q29" s="139" t="s">
         <v>285</v>
       </c>
@@ -19327,11 +19324,11 @@
       <c r="N31" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O31" s="923" t="str">
+      <c r="O31" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD30:AD31),0),"")</f>
         <v/>
       </c>
-      <c r="P31" s="924"/>
+      <c r="P31" s="925"/>
       <c r="Q31" s="138" t="s">
         <v>33</v>
       </c>
@@ -19392,11 +19389,11 @@
       <c r="N32" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O32" s="921" t="str">
+      <c r="O32" s="922" t="str">
         <f ca="1">IF(O31="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD30,AD31,AD32),0),TRUNC(AVERAGE(AD30,AD31,AD32),0)))</f>
         <v/>
       </c>
-      <c r="P32" s="922"/>
+      <c r="P32" s="923"/>
       <c r="Q32" s="139" t="s">
         <v>285</v>
       </c>
@@ -19520,11 +19517,11 @@
       <c r="N34" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O34" s="923" t="str">
+      <c r="O34" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD33:AD34),0),"")</f>
         <v/>
       </c>
-      <c r="P34" s="924"/>
+      <c r="P34" s="925"/>
       <c r="Q34" s="138" t="s">
         <v>33</v>
       </c>
@@ -19585,11 +19582,11 @@
       <c r="N35" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O35" s="921" t="str">
+      <c r="O35" s="922" t="str">
         <f ca="1">IF(O34="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD33,AD34,AD35),0),TRUNC(AVERAGE(AD33,AD34,AD35),0)))</f>
         <v/>
       </c>
-      <c r="P35" s="922"/>
+      <c r="P35" s="923"/>
       <c r="Q35" s="139" t="s">
         <v>285</v>
       </c>
@@ -19713,11 +19710,11 @@
       <c r="N37" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O37" s="923" t="str">
+      <c r="O37" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD36:AD37),0),"")</f>
         <v/>
       </c>
-      <c r="P37" s="924"/>
+      <c r="P37" s="925"/>
       <c r="Q37" s="138" t="s">
         <v>33</v>
       </c>
@@ -19778,11 +19775,11 @@
       <c r="N38" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O38" s="921" t="str">
+      <c r="O38" s="922" t="str">
         <f ca="1">IF(O37="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD36,AD37,AD38),0),TRUNC(AVERAGE(AD36,AD37,AD38),0)))</f>
         <v/>
       </c>
-      <c r="P38" s="922"/>
+      <c r="P38" s="923"/>
       <c r="Q38" s="139" t="s">
         <v>285</v>
       </c>
@@ -19906,11 +19903,11 @@
       <c r="N40" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O40" s="923" t="str">
+      <c r="O40" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD39:AD40),0),"")</f>
         <v/>
       </c>
-      <c r="P40" s="924"/>
+      <c r="P40" s="925"/>
       <c r="Q40" s="138" t="s">
         <v>33</v>
       </c>
@@ -19971,11 +19968,11 @@
       <c r="N41" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O41" s="921" t="str">
+      <c r="O41" s="922" t="str">
         <f ca="1">IF(O40="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD39,AD40,AD41),0),TRUNC(AVERAGE(AD39,AD40,AD41),0)))</f>
         <v/>
       </c>
-      <c r="P41" s="922"/>
+      <c r="P41" s="923"/>
       <c r="Q41" s="139" t="s">
         <v>285</v>
       </c>
@@ -20099,11 +20096,11 @@
       <c r="N43" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O43" s="923" t="str">
+      <c r="O43" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD42:AD43),0),"")</f>
         <v/>
       </c>
-      <c r="P43" s="924"/>
+      <c r="P43" s="925"/>
       <c r="Q43" s="138" t="s">
         <v>33</v>
       </c>
@@ -20164,11 +20161,11 @@
       <c r="N44" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O44" s="921" t="str">
+      <c r="O44" s="922" t="str">
         <f ca="1">IF(O43="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD42,AD43,AD44),0),TRUNC(AVERAGE(AD42,AD43,AD44),0)))</f>
         <v/>
       </c>
-      <c r="P44" s="922"/>
+      <c r="P44" s="923"/>
       <c r="Q44" s="139" t="s">
         <v>285</v>
       </c>
@@ -20292,11 +20289,11 @@
       <c r="N46" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="O46" s="923" t="str">
+      <c r="O46" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD45:AD46),0),"")</f>
         <v/>
       </c>
-      <c r="P46" s="924"/>
+      <c r="P46" s="925"/>
       <c r="Q46" s="138" t="s">
         <v>33</v>
       </c>
@@ -20357,11 +20354,11 @@
       <c r="N47" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="O47" s="921" t="str">
+      <c r="O47" s="922" t="str">
         <f ca="1">IF(O46="","",IF(#REF!="Non validé",0.9*IF(AnalysesComparatives!$H$17="Oui",TRUNC(AVERAGE(AD45,AD46,AD47),0),TRUNC(AVERAGE(AD45,AD46),0)),IF(AnalysesComparatives!$H$17="Oui",TRUNC(AVERAGE(AD45,AD46,AD47),0),TRUNC(AVERAGE(AD45,AD46),0))))</f>
         <v/>
       </c>
-      <c r="P47" s="922"/>
+      <c r="P47" s="923"/>
       <c r="Q47" s="139" t="s">
         <v>285</v>
       </c>
@@ -20482,11 +20479,11 @@
       </c>
     </row>
     <row r="49" spans="15:30" ht="13" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="O49" s="923" t="str">
+      <c r="O49" s="924" t="str">
         <f ca="1">IFERROR(TRUNC(AVERAGE(AD48:AD49),0),"")</f>
         <v/>
       </c>
-      <c r="P49" s="924"/>
+      <c r="P49" s="925"/>
       <c r="Q49" s="108" t="s">
         <v>33</v>
       </c>
@@ -20544,11 +20541,11 @@
       </c>
     </row>
     <row r="50" spans="15:30" ht="13" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="O50" s="921" t="str">
+      <c r="O50" s="922" t="str">
         <f ca="1">IF(O49="","",IF(#REF!="Non validé",0.9*TRUNC(AVERAGE(AD48,AD49,AD50),0),TRUNC(AVERAGE(AD48,AD49,AD50),0)))</f>
         <v/>
       </c>
-      <c r="P50" s="926"/>
+      <c r="P50" s="927"/>
       <c r="Q50" s="139" t="s">
         <v>285</v>
       </c>
@@ -21376,11 +21373,11 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="33" x14ac:dyDescent="0.4">
-      <c r="A25" s="927" t="s">
+      <c r="A25" s="928" t="s">
         <v>239</v>
       </c>
-      <c r="B25" s="927"/>
-      <c r="C25" s="927"/>
+      <c r="B25" s="928"/>
+      <c r="C25" s="928"/>
     </row>
     <row r="30" spans="1:15" s="157" customFormat="1" ht="68" x14ac:dyDescent="0.4">
       <c r="A30" s="154"/>
@@ -21864,11 +21861,11 @@
       </c>
     </row>
     <row r="46" spans="1:15" ht="33" x14ac:dyDescent="0.4">
-      <c r="A46" s="927" t="s">
+      <c r="A46" s="928" t="s">
         <v>240</v>
       </c>
-      <c r="B46" s="927"/>
-      <c r="C46" s="927"/>
+      <c r="B46" s="928"/>
+      <c r="C46" s="928"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A47" s="159" t="s">
@@ -23171,119 +23168,119 @@
     </row>
     <row r="26" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="40"/>
-      <c r="B26" s="928" t="s">
+      <c r="B26" s="929" t="s">
         <v>300</v>
       </c>
-      <c r="C26" s="928"/>
-      <c r="D26" s="928"/>
-      <c r="E26" s="928"/>
-      <c r="F26" s="928"/>
-      <c r="G26" s="928"/>
-      <c r="H26" s="928"/>
-      <c r="I26" s="928"/>
-      <c r="J26" s="928"/>
+      <c r="C26" s="929"/>
+      <c r="D26" s="929"/>
+      <c r="E26" s="929"/>
+      <c r="F26" s="929"/>
+      <c r="G26" s="929"/>
+      <c r="H26" s="929"/>
+      <c r="I26" s="929"/>
+      <c r="J26" s="929"/>
       <c r="K26" s="40"/>
     </row>
     <row r="27" spans="1:11" ht="12.7" x14ac:dyDescent="0.4">
       <c r="A27" s="40"/>
-      <c r="B27" s="928"/>
-      <c r="C27" s="928"/>
-      <c r="D27" s="928"/>
-      <c r="E27" s="928"/>
-      <c r="F27" s="928"/>
-      <c r="G27" s="928"/>
-      <c r="H27" s="928"/>
-      <c r="I27" s="928"/>
-      <c r="J27" s="928"/>
+      <c r="B27" s="929"/>
+      <c r="C27" s="929"/>
+      <c r="D27" s="929"/>
+      <c r="E27" s="929"/>
+      <c r="F27" s="929"/>
+      <c r="G27" s="929"/>
+      <c r="H27" s="929"/>
+      <c r="I27" s="929"/>
+      <c r="J27" s="929"/>
       <c r="K27" s="40"/>
     </row>
     <row r="35" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D35" s="929"/>
-      <c r="E35" s="930"/>
-      <c r="F35" s="930"/>
-      <c r="G35" s="930"/>
-      <c r="H35" s="930"/>
-      <c r="I35" s="930"/>
+      <c r="D35" s="930"/>
+      <c r="E35" s="931"/>
+      <c r="F35" s="931"/>
+      <c r="G35" s="931"/>
+      <c r="H35" s="931"/>
+      <c r="I35" s="931"/>
     </row>
     <row r="36" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D36" s="930"/>
-      <c r="E36" s="930"/>
-      <c r="F36" s="930"/>
-      <c r="G36" s="930"/>
-      <c r="H36" s="930"/>
-      <c r="I36" s="930"/>
+      <c r="D36" s="931"/>
+      <c r="E36" s="931"/>
+      <c r="F36" s="931"/>
+      <c r="G36" s="931"/>
+      <c r="H36" s="931"/>
+      <c r="I36" s="931"/>
     </row>
     <row r="37" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D37" s="930"/>
-      <c r="E37" s="930"/>
-      <c r="F37" s="930"/>
-      <c r="G37" s="930"/>
-      <c r="H37" s="930"/>
-      <c r="I37" s="930"/>
+      <c r="D37" s="931"/>
+      <c r="E37" s="931"/>
+      <c r="F37" s="931"/>
+      <c r="G37" s="931"/>
+      <c r="H37" s="931"/>
+      <c r="I37" s="931"/>
     </row>
     <row r="38" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D38" s="930"/>
-      <c r="E38" s="930"/>
-      <c r="F38" s="930"/>
-      <c r="G38" s="930"/>
-      <c r="H38" s="930"/>
-      <c r="I38" s="930"/>
+      <c r="D38" s="931"/>
+      <c r="E38" s="931"/>
+      <c r="F38" s="931"/>
+      <c r="G38" s="931"/>
+      <c r="H38" s="931"/>
+      <c r="I38" s="931"/>
     </row>
     <row r="39" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D39" s="930"/>
-      <c r="E39" s="930"/>
-      <c r="F39" s="930"/>
-      <c r="G39" s="930"/>
-      <c r="H39" s="930"/>
-      <c r="I39" s="930"/>
+      <c r="D39" s="931"/>
+      <c r="E39" s="931"/>
+      <c r="F39" s="931"/>
+      <c r="G39" s="931"/>
+      <c r="H39" s="931"/>
+      <c r="I39" s="931"/>
     </row>
     <row r="40" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D40" s="930"/>
-      <c r="E40" s="930"/>
-      <c r="F40" s="930"/>
-      <c r="G40" s="930"/>
-      <c r="H40" s="930"/>
-      <c r="I40" s="930"/>
+      <c r="D40" s="931"/>
+      <c r="E40" s="931"/>
+      <c r="F40" s="931"/>
+      <c r="G40" s="931"/>
+      <c r="H40" s="931"/>
+      <c r="I40" s="931"/>
     </row>
     <row r="41" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D41" s="930"/>
-      <c r="E41" s="930"/>
-      <c r="F41" s="930"/>
-      <c r="G41" s="930"/>
-      <c r="H41" s="930"/>
-      <c r="I41" s="930"/>
+      <c r="D41" s="931"/>
+      <c r="E41" s="931"/>
+      <c r="F41" s="931"/>
+      <c r="G41" s="931"/>
+      <c r="H41" s="931"/>
+      <c r="I41" s="931"/>
     </row>
     <row r="42" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D42" s="930"/>
-      <c r="E42" s="930"/>
-      <c r="F42" s="930"/>
-      <c r="G42" s="930"/>
-      <c r="H42" s="930"/>
-      <c r="I42" s="930"/>
+      <c r="D42" s="931"/>
+      <c r="E42" s="931"/>
+      <c r="F42" s="931"/>
+      <c r="G42" s="931"/>
+      <c r="H42" s="931"/>
+      <c r="I42" s="931"/>
     </row>
     <row r="43" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D43" s="930"/>
-      <c r="E43" s="930"/>
-      <c r="F43" s="930"/>
-      <c r="G43" s="930"/>
-      <c r="H43" s="930"/>
-      <c r="I43" s="930"/>
+      <c r="D43" s="931"/>
+      <c r="E43" s="931"/>
+      <c r="F43" s="931"/>
+      <c r="G43" s="931"/>
+      <c r="H43" s="931"/>
+      <c r="I43" s="931"/>
     </row>
     <row r="44" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D44" s="930"/>
-      <c r="E44" s="930"/>
-      <c r="F44" s="930"/>
-      <c r="G44" s="930"/>
-      <c r="H44" s="930"/>
-      <c r="I44" s="930"/>
+      <c r="D44" s="931"/>
+      <c r="E44" s="931"/>
+      <c r="F44" s="931"/>
+      <c r="G44" s="931"/>
+      <c r="H44" s="931"/>
+      <c r="I44" s="931"/>
     </row>
     <row r="45" spans="4:9" ht="12.7" hidden="1" x14ac:dyDescent="0.4">
-      <c r="D45" s="930"/>
-      <c r="E45" s="930"/>
-      <c r="F45" s="930"/>
-      <c r="G45" s="930"/>
-      <c r="H45" s="930"/>
-      <c r="I45" s="930"/>
+      <c r="D45" s="931"/>
+      <c r="E45" s="931"/>
+      <c r="F45" s="931"/>
+      <c r="G45" s="931"/>
+      <c r="H45" s="931"/>
+      <c r="I45" s="931"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -40824,7 +40821,7 @@
       <c r="A23" s="209"/>
       <c r="B23" s="209"/>
       <c r="C23" s="730" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D23" s="731"/>
       <c r="E23" s="731"/>
@@ -41965,7 +41962,7 @@
       <pane xSplit="1" ySplit="7" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="J33" sqref="J33:K33"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="12.7" outlineLevelRow="2" x14ac:dyDescent="0.4"/>
@@ -41990,26 +41987,26 @@
     <row r="1" spans="2:123" s="267" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B1" s="483"/>
       <c r="C1" s="13"/>
-      <c r="D1" s="869" t="s">
+      <c r="D1" s="870" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="870"/>
-      <c r="F1" s="870"/>
-      <c r="G1" s="870"/>
-      <c r="H1" s="870"/>
-      <c r="I1" s="870"/>
-      <c r="J1" s="870"/>
-      <c r="K1" s="870"/>
-      <c r="L1" s="870"/>
-      <c r="M1" s="871"/>
+      <c r="E1" s="871"/>
+      <c r="F1" s="871"/>
+      <c r="G1" s="871"/>
+      <c r="H1" s="871"/>
+      <c r="I1" s="871"/>
+      <c r="J1" s="871"/>
+      <c r="K1" s="871"/>
+      <c r="L1" s="871"/>
+      <c r="M1" s="872"/>
     </row>
     <row r="2" spans="2:123" ht="22.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="484"/>
       <c r="C2"/>
-      <c r="D2" s="867" t="s">
+      <c r="D2" s="868" t="s">
         <v>334</v>
       </c>
-      <c r="E2" s="868"/>
+      <c r="E2" s="869"/>
       <c r="F2" s="790"/>
       <c r="G2" s="791"/>
       <c r="H2" s="791"/>
@@ -42040,18 +42037,18 @@
     <row r="3" spans="2:123" s="359" customFormat="1" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="485"/>
       <c r="C3"/>
-      <c r="D3" s="861" t="s">
-        <v>336</v>
-      </c>
-      <c r="E3" s="862"/>
-      <c r="F3" s="865"/>
-      <c r="G3" s="865"/>
-      <c r="H3" s="863" t="s">
+      <c r="D3" s="862" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="863"/>
+      <c r="F3" s="866"/>
+      <c r="G3" s="866"/>
+      <c r="H3" s="864" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="864"/>
-      <c r="J3" s="866"/>
-      <c r="K3" s="866"/>
+      <c r="I3" s="865"/>
+      <c r="J3" s="867"/>
+      <c r="K3" s="867"/>
       <c r="L3" s="495" t="s">
         <v>4</v>
       </c>
@@ -42060,18 +42057,18 @@
     <row r="4" spans="2:123" s="403" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="486"/>
       <c r="C4"/>
-      <c r="D4" s="861" t="s">
-        <v>389</v>
-      </c>
-      <c r="E4" s="862"/>
-      <c r="F4" s="891"/>
-      <c r="G4" s="891"/>
-      <c r="H4" s="862" t="s">
-        <v>397</v>
-      </c>
-      <c r="I4" s="862"/>
-      <c r="J4" s="866"/>
-      <c r="K4" s="866"/>
+      <c r="D4" s="862" t="s">
+        <v>388</v>
+      </c>
+      <c r="E4" s="863"/>
+      <c r="F4" s="892"/>
+      <c r="G4" s="892"/>
+      <c r="H4" s="863" t="s">
+        <v>396</v>
+      </c>
+      <c r="I4" s="863"/>
+      <c r="J4" s="867"/>
+      <c r="K4" s="867"/>
       <c r="L4" s="495" t="s">
         <v>6</v>
       </c>
@@ -42082,18 +42079,18 @@
       <c r="C5" t="s">
         <v>234</v>
       </c>
-      <c r="D5" s="889" t="s">
-        <v>390</v>
-      </c>
-      <c r="E5" s="890"/>
-      <c r="F5" s="891"/>
-      <c r="G5" s="891"/>
-      <c r="H5" s="901" t="s">
-        <v>396</v>
-      </c>
-      <c r="I5" s="902"/>
-      <c r="J5" s="866"/>
-      <c r="K5" s="866"/>
+      <c r="D5" s="890" t="s">
+        <v>389</v>
+      </c>
+      <c r="E5" s="891"/>
+      <c r="F5" s="892"/>
+      <c r="G5" s="892"/>
+      <c r="H5" s="902" t="s">
+        <v>395</v>
+      </c>
+      <c r="I5" s="903"/>
+      <c r="J5" s="867"/>
+      <c r="K5" s="867"/>
       <c r="L5" s="464" t="s">
         <v>7</v>
       </c>
@@ -42101,18 +42098,18 @@
     </row>
     <row r="6" spans="2:123" s="403" customFormat="1" ht="22.7" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="486"/>
-      <c r="D6" s="889" t="s">
-        <v>400</v>
-      </c>
-      <c r="E6" s="890"/>
-      <c r="F6" s="891"/>
-      <c r="G6" s="891"/>
-      <c r="H6" s="862" t="s">
-        <v>398</v>
-      </c>
-      <c r="I6" s="862"/>
-      <c r="J6" s="866"/>
-      <c r="K6" s="866"/>
+      <c r="D6" s="890" t="s">
+        <v>399</v>
+      </c>
+      <c r="E6" s="891"/>
+      <c r="F6" s="892"/>
+      <c r="G6" s="892"/>
+      <c r="H6" s="863" t="s">
+        <v>397</v>
+      </c>
+      <c r="I6" s="863"/>
+      <c r="J6" s="867"/>
+      <c r="K6" s="867"/>
       <c r="L6" s="794"/>
       <c r="M6" s="795"/>
       <c r="N6" s="459"/>
@@ -42124,7 +42121,7 @@
       <c r="F7" s="788"/>
       <c r="G7" s="789"/>
       <c r="H7" s="787" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I7" s="787"/>
       <c r="J7" s="793"/>
@@ -42146,7 +42143,7 @@
     <row r="9" spans="2:123" s="305" customFormat="1" ht="37.700000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B9" s="469"/>
       <c r="D9" s="801" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E9" s="802"/>
       <c r="F9" s="802"/>
@@ -42161,13 +42158,13 @@
     <row r="10" spans="2:123" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B10" s="469"/>
       <c r="D10" s="835" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E10" s="835"/>
       <c r="F10" s="839"/>
       <c r="G10" s="839"/>
       <c r="H10" s="837" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I10" s="837"/>
       <c r="J10" s="431"/>
@@ -42176,13 +42173,13 @@
     <row r="11" spans="2:123" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B11" s="469"/>
       <c r="D11" s="836" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E11" s="836"/>
       <c r="F11" s="840"/>
       <c r="G11" s="840"/>
       <c r="H11" s="838" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I11" s="838"/>
       <c r="J11" s="431"/>
@@ -42191,13 +42188,13 @@
     <row r="12" spans="2:123" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B12" s="469"/>
       <c r="D12" s="836" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E12" s="836"/>
       <c r="F12" s="840"/>
       <c r="G12" s="840"/>
       <c r="H12" s="838" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I12" s="838"/>
       <c r="J12" s="431"/>
@@ -42206,13 +42203,13 @@
     <row r="13" spans="2:123" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B13" s="469"/>
       <c r="D13" s="836" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E13" s="836"/>
       <c r="F13" s="840"/>
       <c r="G13" s="840"/>
       <c r="H13" s="838" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I13" s="838"/>
       <c r="J13" s="431"/>
@@ -42235,7 +42232,7 @@
     <row r="15" spans="2:123" s="305" customFormat="1" ht="21" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="469"/>
       <c r="D15" s="448" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E15" s="444"/>
       <c r="F15" s="444"/>
@@ -42254,35 +42251,35 @@
     <row r="17" spans="2:14" s="305" customFormat="1" ht="46.1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="469"/>
       <c r="D17" s="815" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E17" s="816"/>
       <c r="F17" s="815" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G17" s="817"/>
       <c r="H17" s="818" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="I17" s="817"/>
       <c r="J17" s="432" t="s">
+        <v>355</v>
+      </c>
+      <c r="K17" s="430" t="s">
         <v>356</v>
       </c>
-      <c r="K17" s="430" t="s">
+      <c r="L17" s="430" t="s">
         <v>357</v>
       </c>
-      <c r="L17" s="430" t="s">
+      <c r="M17" s="470" t="s">
         <v>358</v>
-      </c>
-      <c r="M17" s="470" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="18" spans="2:14" s="305" customFormat="1" ht="24.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="469"/>
       <c r="D18" s="830"/>
       <c r="E18" s="831"/>
-      <c r="F18" s="931"/>
+      <c r="F18" s="841"/>
       <c r="G18" s="829"/>
       <c r="H18" s="828"/>
       <c r="I18" s="829"/>
@@ -42307,7 +42304,7 @@
     <row r="20" spans="2:14" s="305" customFormat="1" ht="35.450000000000003" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="469"/>
       <c r="D20" s="832" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E20" s="833"/>
       <c r="F20" s="833"/>
@@ -42326,7 +42323,7 @@
     <row r="22" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B22" s="469"/>
       <c r="D22" s="827" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E22" s="804"/>
       <c r="F22" s="804">
@@ -42341,7 +42338,7 @@
         <v>3</v>
       </c>
       <c r="K22" s="804" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L22" s="804"/>
       <c r="M22" s="822"/>
@@ -42349,7 +42346,7 @@
     <row r="23" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B23" s="469"/>
       <c r="D23" s="813" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E23" s="814"/>
       <c r="F23" s="826"/>
@@ -42367,7 +42364,7 @@
     <row r="24" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B24" s="469"/>
       <c r="D24" s="819" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E24" s="820"/>
       <c r="F24" s="821" t="str">
@@ -42406,18 +42403,18 @@
     </row>
     <row r="26" spans="2:14" s="305" customFormat="1" ht="32.450000000000003" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="469"/>
-      <c r="D26" s="874" t="s">
-        <v>364</v>
-      </c>
-      <c r="E26" s="875"/>
-      <c r="F26" s="875"/>
-      <c r="G26" s="875"/>
-      <c r="H26" s="875"/>
-      <c r="I26" s="875"/>
-      <c r="J26" s="875"/>
-      <c r="K26" s="875"/>
-      <c r="L26" s="875"/>
-      <c r="M26" s="876"/>
+      <c r="D26" s="875" t="s">
+        <v>363</v>
+      </c>
+      <c r="E26" s="876"/>
+      <c r="F26" s="876"/>
+      <c r="G26" s="876"/>
+      <c r="H26" s="876"/>
+      <c r="I26" s="876"/>
+      <c r="J26" s="876"/>
+      <c r="K26" s="876"/>
+      <c r="L26" s="876"/>
+      <c r="M26" s="877"/>
     </row>
     <row r="27" spans="2:14" s="305" customFormat="1" ht="11.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B27" s="469"/>
@@ -42426,7 +42423,7 @@
     <row r="28" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B28" s="469"/>
       <c r="D28" s="814" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E28" s="814"/>
       <c r="F28" s="814"/>
@@ -42440,78 +42437,78 @@
     <row r="29" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B29" s="469"/>
       <c r="D29" s="814" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E29" s="814"/>
       <c r="F29" s="814"/>
       <c r="G29" s="814"/>
       <c r="H29" s="814"/>
       <c r="I29" s="814"/>
-      <c r="J29" s="846"/>
-      <c r="K29" s="846"/>
+      <c r="J29" s="847"/>
+      <c r="K29" s="847"/>
       <c r="M29" s="466"/>
     </row>
     <row r="30" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B30" s="469"/>
       <c r="D30" s="814" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E30" s="814"/>
       <c r="F30" s="814"/>
       <c r="G30" s="814"/>
       <c r="H30" s="814"/>
       <c r="I30" s="814"/>
-      <c r="J30" s="847" t="e">
+      <c r="J30" s="848" t="e">
         <f>TRUNC(J29/J28,0)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K30" s="847"/>
+      <c r="K30" s="848"/>
       <c r="M30" s="466"/>
     </row>
     <row r="31" spans="2:14" s="305" customFormat="1" ht="16.100000000000001" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B31" s="469"/>
       <c r="D31" s="814" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E31" s="814"/>
       <c r="F31" s="814"/>
       <c r="G31" s="814"/>
       <c r="H31" s="814"/>
       <c r="I31" s="814"/>
-      <c r="J31" s="848"/>
-      <c r="K31" s="848"/>
+      <c r="J31" s="849"/>
+      <c r="K31" s="849"/>
       <c r="M31" s="466"/>
       <c r="N31" s="433"/>
     </row>
     <row r="32" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B32" s="469"/>
       <c r="D32" s="814" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E32" s="814"/>
       <c r="F32" s="814"/>
       <c r="G32" s="814"/>
       <c r="H32" s="814"/>
       <c r="I32" s="814"/>
-      <c r="J32" s="886"/>
-      <c r="K32" s="886"/>
+      <c r="J32" s="887"/>
+      <c r="K32" s="887"/>
       <c r="M32" s="466"/>
     </row>
     <row r="33" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B33" s="469"/>
-      <c r="D33" s="845" t="s">
-        <v>370</v>
-      </c>
-      <c r="E33" s="845"/>
-      <c r="F33" s="845"/>
-      <c r="G33" s="845"/>
-      <c r="H33" s="845"/>
-      <c r="I33" s="845"/>
-      <c r="J33" s="847" t="e">
+      <c r="D33" s="846" t="s">
+        <v>369</v>
+      </c>
+      <c r="E33" s="846"/>
+      <c r="F33" s="846"/>
+      <c r="G33" s="846"/>
+      <c r="H33" s="846"/>
+      <c r="I33" s="846"/>
+      <c r="J33" s="848" t="e">
         <f>J30/J31</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K33" s="847"/>
+      <c r="K33" s="848"/>
       <c r="M33" s="466"/>
     </row>
     <row r="34" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -42529,18 +42526,18 @@
     </row>
     <row r="35" spans="2:14" s="305" customFormat="1" ht="21.75" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B35" s="469"/>
-      <c r="D35" s="849" t="s">
-        <v>371</v>
-      </c>
-      <c r="E35" s="850"/>
-      <c r="F35" s="850"/>
-      <c r="G35" s="850"/>
-      <c r="H35" s="850"/>
-      <c r="I35" s="850"/>
-      <c r="J35" s="850"/>
-      <c r="K35" s="850"/>
-      <c r="L35" s="850"/>
-      <c r="M35" s="851"/>
+      <c r="D35" s="850" t="s">
+        <v>370</v>
+      </c>
+      <c r="E35" s="851"/>
+      <c r="F35" s="851"/>
+      <c r="G35" s="851"/>
+      <c r="H35" s="851"/>
+      <c r="I35" s="851"/>
+      <c r="J35" s="851"/>
+      <c r="K35" s="851"/>
+      <c r="L35" s="851"/>
+      <c r="M35" s="852"/>
     </row>
     <row r="36" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B36" s="469"/>
@@ -42549,15 +42546,15 @@
     <row r="37" spans="2:14" s="305" customFormat="1" ht="27" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B37" s="469"/>
       <c r="D37" s="812" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E37" s="812"/>
       <c r="F37" s="812" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G37" s="812"/>
       <c r="H37" s="812" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I37" s="812"/>
       <c r="J37" s="475"/>
@@ -42566,15 +42563,15 @@
     </row>
     <row r="38" spans="2:14" s="305" customFormat="1" ht="19.7" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B38" s="469"/>
-      <c r="D38" s="880"/>
-      <c r="E38" s="880"/>
-      <c r="F38" s="881"/>
-      <c r="G38" s="881"/>
-      <c r="H38" s="882" t="e">
+      <c r="D38" s="881"/>
+      <c r="E38" s="881"/>
+      <c r="F38" s="882"/>
+      <c r="G38" s="882"/>
+      <c r="H38" s="883" t="e">
         <f>(D38-F38)/F38</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I38" s="882"/>
+      <c r="I38" s="883"/>
       <c r="J38" s="435"/>
       <c r="K38" s="476"/>
       <c r="M38" s="466"/>
@@ -42595,18 +42592,18 @@
     </row>
     <row r="40" spans="2:14" s="305" customFormat="1" ht="25.7" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B40" s="469"/>
-      <c r="D40" s="849" t="s">
-        <v>372</v>
-      </c>
-      <c r="E40" s="850"/>
-      <c r="F40" s="850"/>
-      <c r="G40" s="850"/>
-      <c r="H40" s="850"/>
-      <c r="I40" s="850"/>
-      <c r="J40" s="850"/>
-      <c r="K40" s="850"/>
-      <c r="L40" s="850"/>
-      <c r="M40" s="851"/>
+      <c r="D40" s="850" t="s">
+        <v>371</v>
+      </c>
+      <c r="E40" s="851"/>
+      <c r="F40" s="851"/>
+      <c r="G40" s="851"/>
+      <c r="H40" s="851"/>
+      <c r="I40" s="851"/>
+      <c r="J40" s="851"/>
+      <c r="K40" s="851"/>
+      <c r="L40" s="851"/>
+      <c r="M40" s="852"/>
     </row>
     <row r="41" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B41" s="469"/>
@@ -42615,15 +42612,15 @@
     <row r="42" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B42" s="469"/>
       <c r="D42" s="812" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E42" s="812"/>
       <c r="F42" s="812" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G42" s="812"/>
       <c r="H42" s="812" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I42" s="812"/>
       <c r="J42" s="436"/>
@@ -42633,16 +42630,16 @@
     </row>
     <row r="43" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B43" s="469"/>
-      <c r="D43" s="887" t="s">
-        <v>382</v>
-      </c>
-      <c r="E43" s="888"/>
+      <c r="D43" s="888" t="s">
+        <v>381</v>
+      </c>
+      <c r="E43" s="889"/>
       <c r="F43" s="812" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G43" s="812"/>
       <c r="H43" s="812" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I43" s="812"/>
       <c r="J43" s="436"/>
@@ -42652,18 +42649,18 @@
     </row>
     <row r="44" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B44" s="469"/>
-      <c r="D44" s="883"/>
-      <c r="E44" s="883"/>
-      <c r="F44" s="884" t="e">
+      <c r="D44" s="884"/>
+      <c r="E44" s="884"/>
+      <c r="F44" s="885" t="e">
         <f>(K18*J30)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G44" s="884"/>
-      <c r="H44" s="885" t="str">
+      <c r="G44" s="885"/>
+      <c r="H44" s="886" t="str">
         <f>IF(D44&gt;0,(D44-F44)/F44,"")</f>
         <v/>
       </c>
-      <c r="I44" s="885"/>
+      <c r="I44" s="886"/>
       <c r="J44" s="436"/>
       <c r="K44" s="436"/>
       <c r="L44" s="478"/>
@@ -42685,24 +42682,24 @@
     </row>
     <row r="46" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="B46" s="469"/>
-      <c r="D46" s="877" t="s">
-        <v>379</v>
-      </c>
-      <c r="E46" s="878"/>
-      <c r="F46" s="878"/>
-      <c r="G46" s="878"/>
-      <c r="H46" s="878"/>
-      <c r="I46" s="878"/>
-      <c r="J46" s="878"/>
-      <c r="K46" s="878"/>
-      <c r="L46" s="878"/>
-      <c r="M46" s="879"/>
+      <c r="D46" s="878" t="s">
+        <v>378</v>
+      </c>
+      <c r="E46" s="879"/>
+      <c r="F46" s="879"/>
+      <c r="G46" s="879"/>
+      <c r="H46" s="879"/>
+      <c r="I46" s="879"/>
+      <c r="J46" s="879"/>
+      <c r="K46" s="879"/>
+      <c r="L46" s="879"/>
+      <c r="M46" s="880"/>
       <c r="N46" s="437"/>
     </row>
     <row r="47" spans="2:14" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B47" s="469"/>
       <c r="D47" s="809" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E47" s="810"/>
       <c r="F47" s="810"/>
@@ -42729,38 +42726,38 @@
     </row>
     <row r="49" spans="2:123" s="305" customFormat="1" ht="28.1" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B49" s="469"/>
-      <c r="D49" s="841" t="s">
+      <c r="D49" s="842" t="s">
+        <v>338</v>
+      </c>
+      <c r="E49" s="843"/>
+      <c r="F49" s="842" t="s">
+        <v>375</v>
+      </c>
+      <c r="G49" s="843"/>
+      <c r="H49" s="842" t="s">
         <v>339</v>
       </c>
-      <c r="E49" s="842"/>
-      <c r="F49" s="841" t="s">
+      <c r="I49" s="843"/>
+      <c r="J49" s="842" t="s">
+        <v>340</v>
+      </c>
+      <c r="K49" s="843"/>
+      <c r="L49" s="805" t="s">
         <v>376</v>
-      </c>
-      <c r="G49" s="842"/>
-      <c r="H49" s="841" t="s">
-        <v>340</v>
-      </c>
-      <c r="I49" s="842"/>
-      <c r="J49" s="841" t="s">
-        <v>341</v>
-      </c>
-      <c r="K49" s="842"/>
-      <c r="L49" s="805" t="s">
-        <v>377</v>
       </c>
       <c r="M49" s="806"/>
       <c r="N49" s="437"/>
     </row>
     <row r="50" spans="2:123" s="305" customFormat="1" ht="23.45" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B50" s="469"/>
-      <c r="D50" s="843"/>
-      <c r="E50" s="844"/>
-      <c r="F50" s="843"/>
-      <c r="G50" s="844"/>
-      <c r="H50" s="843"/>
-      <c r="I50" s="844"/>
-      <c r="J50" s="843"/>
-      <c r="K50" s="844"/>
+      <c r="D50" s="844"/>
+      <c r="E50" s="845"/>
+      <c r="F50" s="844"/>
+      <c r="G50" s="845"/>
+      <c r="H50" s="844"/>
+      <c r="I50" s="845"/>
+      <c r="J50" s="844"/>
+      <c r="K50" s="845"/>
       <c r="L50" s="807" t="str">
         <f>IF(AND(J50&lt;=8,J50&gt;=2),"Oui","Non")</f>
         <v>Non</v>
@@ -42785,7 +42782,7 @@
     <row r="53" spans="2:123" s="305" customFormat="1" ht="40.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B53" s="469"/>
       <c r="D53" s="801" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E53" s="802"/>
       <c r="F53" s="802"/>
@@ -42821,13 +42818,13 @@
     </row>
     <row r="56" spans="2:123" s="305" customFormat="1" ht="15" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B56" s="469"/>
-      <c r="D56" s="872"/>
-      <c r="E56" s="872"/>
-      <c r="F56" s="872"/>
-      <c r="G56" s="872"/>
-      <c r="H56" s="872"/>
-      <c r="I56" s="872"/>
-      <c r="J56" s="873"/>
+      <c r="D56" s="873"/>
+      <c r="E56" s="873"/>
+      <c r="F56" s="873"/>
+      <c r="G56" s="873"/>
+      <c r="H56" s="873"/>
+      <c r="I56" s="873"/>
+      <c r="J56" s="874"/>
       <c r="M56" s="466"/>
     </row>
     <row r="57" spans="2:123" s="305" customFormat="1" ht="33" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.55000000000000004">
@@ -42853,10 +42850,10 @@
       <c r="E58" s="442"/>
       <c r="F58" s="449"/>
       <c r="G58" s="449"/>
-      <c r="H58" s="918" t="s">
+      <c r="H58" s="919" t="s">
         <v>12</v>
       </c>
-      <c r="I58" s="852"/>
+      <c r="I58" s="853"/>
       <c r="J58" s="310" t="s">
         <v>48</v>
       </c>
@@ -42870,14 +42867,14 @@
       <c r="D59" s="313">
         <v>0</v>
       </c>
-      <c r="E59" s="856" t="str">
+      <c r="E59" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D59+2,FALSE),"")</f>
         <v>Prélèvement sur un point présentant un écoulement permanent (entrée/sortie) ?</v>
       </c>
-      <c r="F59" s="856"/>
-      <c r="G59" s="856"/>
-      <c r="H59" s="859"/>
-      <c r="I59" s="860"/>
+      <c r="F59" s="857"/>
+      <c r="G59" s="857"/>
+      <c r="H59" s="860"/>
+      <c r="I59" s="861"/>
       <c r="J59" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D59+2,FALSE),"")</f>
         <v>0</v>
@@ -42894,14 +42891,14 @@
       <c r="D60" s="320">
         <v>1</v>
       </c>
-      <c r="E60" s="856" t="str">
+      <c r="E60" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D60+2,FALSE),"")</f>
         <v>L'accès à l'ouvrage et aux équipements de mesure se fait-il en toute sécurité pour les agents en charge des opérations de contrôles et d'entretien... ?</v>
       </c>
-      <c r="F60" s="856"/>
-      <c r="G60" s="856"/>
-      <c r="H60" s="857"/>
-      <c r="I60" s="858"/>
+      <c r="F60" s="857"/>
+      <c r="G60" s="857"/>
+      <c r="H60" s="858"/>
+      <c r="I60" s="859"/>
       <c r="J60" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D60+2,FALSE),"")</f>
         <v>5</v>
@@ -42919,14 +42916,14 @@
       <c r="D61" s="320">
         <v>2</v>
       </c>
-      <c r="E61" s="856" t="str">
+      <c r="E61" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D61+2,FALSE),"")</f>
         <v>Le point de prélèvement est-il correctement implanté et situé dans un milieu homogène et brassé ?</v>
       </c>
-      <c r="F61" s="856"/>
-      <c r="G61" s="856"/>
-      <c r="H61" s="857"/>
-      <c r="I61" s="858"/>
+      <c r="F61" s="857"/>
+      <c r="G61" s="857"/>
+      <c r="H61" s="858"/>
+      <c r="I61" s="859"/>
       <c r="J61" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D61+2,FALSE),"")</f>
         <v>20</v>
@@ -42953,14 +42950,14 @@
       <c r="D62" s="320">
         <v>3</v>
       </c>
-      <c r="E62" s="856" t="str">
+      <c r="E62" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D62+2,FALSE),"")</f>
         <v>Le circuit de prélèvement, y compris la boucle primaire, présente t-il un état de fonctionnement satisfaisant, son diamètre est-il ≥ à 9 mm ?</v>
       </c>
-      <c r="F62" s="856"/>
-      <c r="G62" s="856"/>
-      <c r="H62" s="857"/>
-      <c r="I62" s="858"/>
+      <c r="F62" s="857"/>
+      <c r="G62" s="857"/>
+      <c r="H62" s="858"/>
+      <c r="I62" s="859"/>
       <c r="J62" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D62+2,FALSE),"")</f>
         <v>5</v>
@@ -42987,14 +42984,14 @@
       <c r="D63" s="320">
         <v>4</v>
       </c>
-      <c r="E63" s="856" t="str">
+      <c r="E63" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D63+2,FALSE),"")</f>
         <v>Le volume de prélèvement par cycle est-il ≥ à 50 ml et est-il répétable à ± 5 % ?</v>
       </c>
-      <c r="F63" s="856"/>
-      <c r="G63" s="856"/>
-      <c r="H63" s="857"/>
-      <c r="I63" s="858"/>
+      <c r="F63" s="857"/>
+      <c r="G63" s="857"/>
+      <c r="H63" s="858"/>
+      <c r="I63" s="859"/>
       <c r="J63" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D63+2,FALSE),"")</f>
         <v>5</v>
@@ -43021,14 +43018,14 @@
       <c r="D64" s="320">
         <v>5</v>
       </c>
-      <c r="E64" s="856" t="str">
+      <c r="E64" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D64+2,FALSE),"")</f>
         <v>La vitesse d'aspiration, y compris celle de la boucle primaire, est-elle de ≥ 0,5 m/s ?</v>
       </c>
-      <c r="F64" s="856"/>
-      <c r="G64" s="856"/>
-      <c r="H64" s="857"/>
-      <c r="I64" s="858"/>
+      <c r="F64" s="857"/>
+      <c r="G64" s="857"/>
+      <c r="H64" s="858"/>
+      <c r="I64" s="859"/>
       <c r="J64" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D64+2,FALSE),"")</f>
         <v>5</v>
@@ -43055,15 +43052,15 @@
       <c r="D65" s="320">
         <v>6</v>
       </c>
-      <c r="E65" s="856" t="str">
+      <c r="E65" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D65+2,FALSE),"")</f>
         <v>Le préleveur est-il asservi au débit, ou au volume écoulé, et assure-t-il un nombre de prélèvements égal, en moyenne, au moins à 6 (*) par heure de rejet effectif ? soit 144 prelevements unitaires par 24h.
 (*) Tolérance de validation à 4/h (soit 96 prélèvements/jour), sur justification particulière (évènement exceptionnel).</v>
       </c>
-      <c r="F65" s="856"/>
-      <c r="G65" s="856"/>
-      <c r="H65" s="857"/>
-      <c r="I65" s="858"/>
+      <c r="F65" s="857"/>
+      <c r="G65" s="857"/>
+      <c r="H65" s="858"/>
+      <c r="I65" s="859"/>
       <c r="J65" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D65+2,FALSE),"")</f>
         <v>15</v>
@@ -43090,14 +43087,14 @@
       <c r="D66" s="320">
         <v>7</v>
       </c>
-      <c r="E66" s="856" t="str">
+      <c r="E66" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D66+2,FALSE),"")</f>
         <v xml:space="preserve"> Les horaires de prélèvement et de totalisation des débits sont-ils synchronisés ?</v>
       </c>
-      <c r="F66" s="856"/>
-      <c r="G66" s="856"/>
-      <c r="H66" s="857"/>
-      <c r="I66" s="858"/>
+      <c r="F66" s="857"/>
+      <c r="G66" s="857"/>
+      <c r="H66" s="858"/>
+      <c r="I66" s="859"/>
       <c r="J66" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D66+2,FALSE),"")</f>
         <v>5</v>
@@ -43124,14 +43121,14 @@
       <c r="D67" s="320">
         <v>8</v>
       </c>
-      <c r="E67" s="856" t="str">
+      <c r="E67" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D67+2,FALSE),"")</f>
         <v>La température de l'enceinte de prélèvement est-elle adaptée? Si elle est réfrigérée, sa température est-elle maîtrisée à 5°C ± 3°C ?</v>
       </c>
-      <c r="F67" s="856"/>
-      <c r="G67" s="856"/>
-      <c r="H67" s="857"/>
-      <c r="I67" s="858"/>
+      <c r="F67" s="857"/>
+      <c r="G67" s="857"/>
+      <c r="H67" s="858"/>
+      <c r="I67" s="859"/>
       <c r="J67" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D67+2,FALSE),"")</f>
         <v>20</v>
@@ -43158,14 +43155,14 @@
       <c r="D68" s="320">
         <v>9</v>
       </c>
-      <c r="E68" s="856" t="str">
+      <c r="E68" s="857" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D68+2,FALSE),"")</f>
         <v>L'écart entre le volume théorique et le volume prélevé est-il ≤ à 10% ?</v>
       </c>
-      <c r="F68" s="856"/>
-      <c r="G68" s="856"/>
-      <c r="H68" s="857"/>
-      <c r="I68" s="858"/>
+      <c r="F68" s="857"/>
+      <c r="G68" s="857"/>
+      <c r="H68" s="858"/>
+      <c r="I68" s="859"/>
       <c r="J68" s="400">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D68+2,FALSE),"")</f>
         <v>20</v>
@@ -43192,14 +43189,14 @@
       <c r="D69" s="320">
         <v>10</v>
       </c>
-      <c r="E69" s="856">
+      <c r="E69" s="857">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$3:$AH$16,$D69+2,FALSE),"")</f>
         <v>0</v>
       </c>
-      <c r="F69" s="856"/>
-      <c r="G69" s="856"/>
-      <c r="H69" s="857"/>
-      <c r="I69" s="858"/>
+      <c r="F69" s="857"/>
+      <c r="G69" s="857"/>
+      <c r="H69" s="858"/>
+      <c r="I69" s="859"/>
       <c r="J69" s="400" t="str">
         <f>IFERROR(HLOOKUP(D$57,TAB_Critères!$B$30:$R$40,$D69+2,FALSE),"")</f>
         <v/>
@@ -43228,11 +43225,11 @@
       </c>
       <c r="E70" s="546"/>
       <c r="F70" s="546"/>
-      <c r="G70" s="852"/>
+      <c r="G70" s="853"/>
       <c r="H70" s="546" t="s">
         <v>51</v>
       </c>
-      <c r="I70" s="852"/>
+      <c r="I70" s="853"/>
       <c r="J70" s="310" t="s">
         <v>52</v>
       </c>
@@ -43252,12 +43249,12 @@
     <row r="71" spans="2:123" ht="38.25" customHeight="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B71" s="484"/>
       <c r="C71" s="489"/>
-      <c r="D71" s="853"/>
-      <c r="E71" s="854"/>
-      <c r="F71" s="854"/>
-      <c r="G71" s="855"/>
-      <c r="H71" s="919"/>
-      <c r="I71" s="920"/>
+      <c r="D71" s="854"/>
+      <c r="E71" s="855"/>
+      <c r="F71" s="855"/>
+      <c r="G71" s="856"/>
+      <c r="H71" s="920"/>
+      <c r="I71" s="921"/>
       <c r="J71" s="294">
         <f>IF(D57="","",IF(D57="Préleveur A3",PARAM!$AD$28,IF((SUMIF(H60:H68,"Validé",J60:J68)+SUMIF(H60:H68,"Validé avec réserve",J60:J68))&gt;100,100,SUMIF(H60:H68,"Validé",J60:J68)+SUMIF(H60:H68,"Validé avec réserve",J60:J68))))</f>
         <v>0</v>
@@ -43308,18 +43305,18 @@
     <row r="74" spans="2:123" ht="37.700000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B74" s="484"/>
       <c r="C74" s="305"/>
-      <c r="D74" s="903" t="s">
+      <c r="D74" s="904" t="s">
         <v>54</v>
       </c>
-      <c r="E74" s="904"/>
-      <c r="F74" s="904"/>
-      <c r="G74" s="904"/>
-      <c r="H74" s="904"/>
-      <c r="I74" s="904"/>
-      <c r="J74" s="904"/>
-      <c r="K74" s="904"/>
-      <c r="L74" s="904"/>
-      <c r="M74" s="905"/>
+      <c r="E74" s="905"/>
+      <c r="F74" s="905"/>
+      <c r="G74" s="905"/>
+      <c r="H74" s="905"/>
+      <c r="I74" s="905"/>
+      <c r="J74" s="905"/>
+      <c r="K74" s="905"/>
+      <c r="L74" s="905"/>
+      <c r="M74" s="906"/>
       <c r="DK74" s="243"/>
       <c r="DL74" s="243"/>
       <c r="DM74" s="243"/>
@@ -43350,26 +43347,26 @@
     <row r="76" spans="2:123" outlineLevel="2" x14ac:dyDescent="0.4">
       <c r="B76" s="484"/>
       <c r="C76" s="305"/>
-      <c r="D76" s="910" t="s">
+      <c r="D76" s="911" t="s">
         <v>75</v>
       </c>
-      <c r="E76" s="913" t="s">
+      <c r="E76" s="914" t="s">
         <v>77</v>
       </c>
-      <c r="F76" s="913" t="s">
+      <c r="F76" s="914" t="s">
+        <v>336</v>
+      </c>
+      <c r="G76" s="916" t="s">
+        <v>78</v>
+      </c>
+      <c r="H76" s="914" t="s">
         <v>337</v>
       </c>
-      <c r="G76" s="915" t="s">
+      <c r="I76" s="916" t="s">
         <v>78</v>
       </c>
-      <c r="H76" s="913" t="s">
-        <v>338</v>
-      </c>
-      <c r="I76" s="915" t="s">
-        <v>78</v>
-      </c>
       <c r="J76" s="457" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K76" s="458" t="s">
         <v>76</v>
@@ -43388,12 +43385,12 @@
     <row r="77" spans="2:123" ht="21" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.5">
       <c r="B77" s="484"/>
       <c r="C77" s="305"/>
-      <c r="D77" s="911"/>
-      <c r="E77" s="914"/>
-      <c r="F77" s="914"/>
-      <c r="G77" s="916"/>
-      <c r="H77" s="914"/>
-      <c r="I77" s="916"/>
+      <c r="D77" s="912"/>
+      <c r="E77" s="915"/>
+      <c r="F77" s="915"/>
+      <c r="G77" s="917"/>
+      <c r="H77" s="915"/>
+      <c r="I77" s="917"/>
       <c r="J77" s="481">
         <f>COUNT(J80:J95)</f>
         <v>0</v>
@@ -43416,16 +43413,16 @@
     <row r="78" spans="2:123" outlineLevel="2" x14ac:dyDescent="0.4">
       <c r="B78" s="484"/>
       <c r="C78" s="305"/>
-      <c r="D78" s="911"/>
-      <c r="E78" s="914"/>
-      <c r="F78" s="914"/>
-      <c r="G78" s="916"/>
-      <c r="H78" s="914"/>
-      <c r="I78" s="916"/>
-      <c r="J78" s="906" t="s">
+      <c r="D78" s="912"/>
+      <c r="E78" s="915"/>
+      <c r="F78" s="915"/>
+      <c r="G78" s="917"/>
+      <c r="H78" s="915"/>
+      <c r="I78" s="917"/>
+      <c r="J78" s="907" t="s">
         <v>79</v>
       </c>
-      <c r="K78" s="908" t="s">
+      <c r="K78" s="909" t="s">
         <v>80</v>
       </c>
       <c r="M78" s="466"/>
@@ -43442,16 +43439,16 @@
     <row r="79" spans="2:123" ht="41.7" customHeight="1" outlineLevel="2" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B79" s="484"/>
       <c r="C79" s="305"/>
-      <c r="D79" s="912"/>
-      <c r="E79" s="907"/>
-      <c r="F79" s="907"/>
-      <c r="G79" s="917"/>
-      <c r="H79" s="907"/>
-      <c r="I79" s="917"/>
-      <c r="J79" s="907"/>
-      <c r="K79" s="909"/>
+      <c r="D79" s="913"/>
+      <c r="E79" s="908"/>
+      <c r="F79" s="908"/>
+      <c r="G79" s="918"/>
+      <c r="H79" s="908"/>
+      <c r="I79" s="918"/>
+      <c r="J79" s="908"/>
+      <c r="K79" s="910"/>
       <c r="L79" s="406" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M79" s="466"/>
       <c r="DK79" s="243"/>
@@ -43486,7 +43483,7 @@
         <v>113</v>
       </c>
       <c r="L80" s="406" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="M80" s="466"/>
       <c r="DK80" s="243"/>
@@ -44006,73 +44003,73 @@
     <row r="100" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B100" s="484"/>
       <c r="D100" s="499" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M100" s="466"/>
     </row>
     <row r="101" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B101" s="484"/>
-      <c r="D101" s="892"/>
-      <c r="E101" s="893"/>
-      <c r="F101" s="893"/>
-      <c r="G101" s="893"/>
-      <c r="H101" s="893"/>
-      <c r="I101" s="893"/>
-      <c r="J101" s="893"/>
-      <c r="K101" s="893"/>
-      <c r="L101" s="894"/>
+      <c r="D101" s="893"/>
+      <c r="E101" s="894"/>
+      <c r="F101" s="894"/>
+      <c r="G101" s="894"/>
+      <c r="H101" s="894"/>
+      <c r="I101" s="894"/>
+      <c r="J101" s="894"/>
+      <c r="K101" s="894"/>
+      <c r="L101" s="895"/>
       <c r="M101" s="466"/>
     </row>
     <row r="102" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B102" s="484"/>
-      <c r="D102" s="895"/>
-      <c r="E102" s="896"/>
-      <c r="F102" s="896"/>
-      <c r="G102" s="896"/>
-      <c r="H102" s="896"/>
-      <c r="I102" s="896"/>
-      <c r="J102" s="896"/>
-      <c r="K102" s="896"/>
-      <c r="L102" s="897"/>
+      <c r="D102" s="896"/>
+      <c r="E102" s="897"/>
+      <c r="F102" s="897"/>
+      <c r="G102" s="897"/>
+      <c r="H102" s="897"/>
+      <c r="I102" s="897"/>
+      <c r="J102" s="897"/>
+      <c r="K102" s="897"/>
+      <c r="L102" s="898"/>
       <c r="M102" s="466"/>
     </row>
     <row r="103" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B103" s="484"/>
-      <c r="D103" s="895"/>
-      <c r="E103" s="896"/>
-      <c r="F103" s="896"/>
-      <c r="G103" s="896"/>
-      <c r="H103" s="896"/>
-      <c r="I103" s="896"/>
-      <c r="J103" s="896"/>
-      <c r="K103" s="896"/>
-      <c r="L103" s="897"/>
+      <c r="D103" s="896"/>
+      <c r="E103" s="897"/>
+      <c r="F103" s="897"/>
+      <c r="G103" s="897"/>
+      <c r="H103" s="897"/>
+      <c r="I103" s="897"/>
+      <c r="J103" s="897"/>
+      <c r="K103" s="897"/>
+      <c r="L103" s="898"/>
       <c r="M103" s="466"/>
     </row>
     <row r="104" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B104" s="484"/>
-      <c r="D104" s="895"/>
-      <c r="E104" s="896"/>
-      <c r="F104" s="896"/>
-      <c r="G104" s="896"/>
-      <c r="H104" s="896"/>
-      <c r="I104" s="896"/>
-      <c r="J104" s="896"/>
-      <c r="K104" s="896"/>
-      <c r="L104" s="897"/>
+      <c r="D104" s="896"/>
+      <c r="E104" s="897"/>
+      <c r="F104" s="897"/>
+      <c r="G104" s="897"/>
+      <c r="H104" s="897"/>
+      <c r="I104" s="897"/>
+      <c r="J104" s="897"/>
+      <c r="K104" s="897"/>
+      <c r="L104" s="898"/>
       <c r="M104" s="466"/>
     </row>
     <row r="105" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B105" s="484"/>
-      <c r="D105" s="898"/>
-      <c r="E105" s="899"/>
-      <c r="F105" s="899"/>
-      <c r="G105" s="899"/>
-      <c r="H105" s="899"/>
-      <c r="I105" s="899"/>
-      <c r="J105" s="899"/>
-      <c r="K105" s="899"/>
-      <c r="L105" s="900"/>
+      <c r="D105" s="899"/>
+      <c r="E105" s="900"/>
+      <c r="F105" s="900"/>
+      <c r="G105" s="900"/>
+      <c r="H105" s="900"/>
+      <c r="I105" s="900"/>
+      <c r="J105" s="900"/>
+      <c r="K105" s="900"/>
+      <c r="L105" s="901"/>
       <c r="M105" s="466"/>
     </row>
     <row r="106" spans="2:13" x14ac:dyDescent="0.4">
@@ -44723,12 +44720,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B79ED2B215C6A64A8EEA6A4A280DADE5" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3888bf875947002d9437d5c56d07b5d3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81251141-7599-4081-9962-8622873f55aa" xmlns:ns3="afd5fb63-b61f-423b-93e7-958e038eacd2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="047a8574d06dd2c3496ab08796c0e7b5" ns2:_="" ns3:_="">
     <xsd:import namespace="81251141-7599-4081-9962-8622873f55aa"/>
@@ -44931,16 +44937,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB702087-7E88-4AF3-B693-D27B95F8995C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA52DDF1-DB9E-4C0C-9E16-F265EDFF44E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -44949,7 +44954,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2814875-A1EC-46C5-A2DA-1FD958EE2B85}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44966,12 +44971,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB702087-7E88-4AF3-B693-D27B95F8995C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>